<commit_message>
fix README.md, add ppt
</commit_message>
<xml_diff>
--- a/api_v0.0.1.xlsx
+++ b/api_v0.0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="History" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>No</t>
   </si>
@@ -145,16 +145,10 @@
     <t>content["name"]</t>
   </si>
   <si>
-    <t>{ cmd:'isexist', result : 0, msg : 'success', content:{userid:userid, users:[user], chats:[chat]} }</t>
-  </si>
-  <si>
     <t>userchanged</t>
   </si>
   <si>
     <t>it's just from server</t>
-  </si>
-  <si>
-    <t>{ cmd:'isexist', result : 0, msg : 'success', content:{users:[user]} }</t>
   </si>
   <si>
     <t>content["from"]</t>
@@ -169,22 +163,37 @@
     <t>content["status"]</t>
   </si>
   <si>
-    <t>{ cmd:'isexist', result : 0, msg : 'success', content:{userid:userid, status:status} }</t>
-  </si>
-  <si>
-    <t>{ cmd:'isexist', result : 0, msg : 'success', content:{from:from, to:to, msg:msg} }</t>
-  </si>
-  <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>{ cmd:'isexist', result : 0, msg : 'success', content:{userid:userid, name:name }</t>
   </si>
   <si>
     <t>time</t>
   </si>
   <si>
-    <t>{ cmd:'isexist', result : 0, msg : 'success', content:yyyyMMddHHmmss }</t>
+    <t>{ cmd:'time', result : 0, msg : 'success', content:yyyyMMddHHmmss }</t>
+  </si>
+  <si>
+    <t>{ cmd:'signup', result : 0, msg : 'success' }</t>
+  </si>
+  <si>
+    <t>{ cmd:'signin', result : 0, msg : 'success', content:{userid:userid, users:[user], chats:[chat]} }</t>
+  </si>
+  <si>
+    <t>{ cmd:'userchanged', result : 0, msg : 'success', content:{users:[user]} }</t>
+  </si>
+  <si>
+    <t>{ cmd:'msg', result : 0, msg : 'success', content:{from:from, to:to, msg:msg} }</t>
+  </si>
+  <si>
+    <t>{ cmd:'status', result : 0, msg : 'success', content:{userid:userid, status:status} }</t>
+  </si>
+  <si>
+    <t>{ cmd:'name', result : 0, msg : 'success', content:{userid:userid, name:name }</t>
+  </si>
+  <si>
+    <t>{ cmd:'signout', result : 0, msg : 'success' }</t>
+  </si>
+  <si>
+    <t>{ cmd:'removeuser', result : 0, msg : 'success' }</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y958"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1213,7 +1222,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="1"/>
@@ -1445,7 +1454,7 @@
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="1"/>
@@ -45074,8 +45083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -45187,15 +45196,15 @@
     </row>
     <row r="5" spans="1:19" ht="37" customHeight="1">
       <c r="B5" s="31" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="28" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="37" customHeight="1">
@@ -45258,7 +45267,7 @@
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="39" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F8" s="26"/>
       <c r="G8" s="1"/>
@@ -45354,7 +45363,7 @@
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="39" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="1"/>
@@ -45420,15 +45429,15 @@
     <row r="15" spans="1:19" ht="37" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="28" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -45454,7 +45463,7 @@
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="39" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F16" s="26"/>
       <c r="G16" s="1"/>
@@ -45475,7 +45484,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="38"/>
       <c r="C17" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="39"/>
@@ -45498,7 +45507,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="38"/>
       <c r="C18" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="39"/>
@@ -45521,7 +45530,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="38"/>
       <c r="C19" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="39"/>
@@ -45550,7 +45559,7 @@
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="39" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="1"/>
@@ -45594,7 +45603,7 @@
       <c r="A22" s="1"/>
       <c r="B22" s="38"/>
       <c r="C22" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="39"/>
@@ -45616,14 +45625,14 @@
     <row r="23" spans="1:19" ht="37" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="38" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="39" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F23" s="26"/>
       <c r="G23" s="1"/>
@@ -45696,7 +45705,7 @@
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="39" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F26" s="26"/>
       <c r="G26" s="1"/>
@@ -45740,7 +45749,7 @@
       <c r="A28" s="1"/>
       <c r="B28" s="38"/>
       <c r="C28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="39"/>
@@ -45769,7 +45778,7 @@
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="39" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="F29" s="26"/>
       <c r="G29" s="1"/>

</xml_diff>